<commit_message>
DAY 3 75% completed
</commit_message>
<xml_diff>
--- a/DS Recordings.xlsx
+++ b/DS Recordings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Tofik\Desktop\INTERNSHIP-BRAINYBEAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220291FD-07EC-4911-A040-B22C01068BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EC9D71-96DF-46B5-8BB9-471A8B9E3F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,9 +420,6 @@
     <t>From predicting customer behavior to optimizing operations, machine learning is transforming industries. Our project, [Project Name], demonstrates how data-driven models can solve . Today, we’ll showcase our methodology, challenges, and how our model enhances efficiency and accuracy</t>
   </si>
   <si>
-    <t>DAY 3</t>
-  </si>
-  <si>
     <t>DAY 4</t>
   </si>
   <si>
@@ -440,7 +437,10 @@
 Conclusion: Summarize findings and provide takeaways.</t>
   </si>
   <si>
-    <t>DAY 2 09-12-2025 TUESDAY</t>
+    <t>DAY 3 10-12-2025 (WEDNESDAY)</t>
+  </si>
+  <si>
+    <t>DAY 2 09-12-2025 (TUESDAY)</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -536,16 +536,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -829,13 +828,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D22"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
     <col min="4" max="4" width="82" customWidth="1"/>
   </cols>
   <sheetData>
@@ -902,12 +902,12 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
@@ -916,7 +916,7 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -930,7 +930,7 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -944,7 +944,7 @@
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -958,7 +958,7 @@
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -972,7 +972,7 @@
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -986,7 +986,7 @@
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -994,30 +994,30 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>2554</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1050,12 +1050,12 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1100,12 +1100,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -1342,7 +1342,7 @@
         <v>98</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1454,7 +1454,7 @@
         <v>121</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Week1 completed week 2 started
</commit_message>
<xml_diff>
--- a/DS Recordings.xlsx
+++ b/DS Recordings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Tofik\Desktop\INTERNSHIP-BRAINYBEAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0C30C9-3DDA-44D4-9C96-6AB3C8F0CFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B230C871-C0CD-4BE4-874A-68FF6E986C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>task_id</t>
   </si>
@@ -437,22 +437,16 @@
     <t>DAY 2 09-12-2025 (TUESDAY)</t>
   </si>
   <si>
-    <t>DAY 6</t>
-  </si>
-  <si>
     <t>DAY 4 11-12-2025 (THURSDAY)</t>
   </si>
   <si>
     <t>DAY 5 12-12-2025 (FRIDAY)</t>
   </si>
   <si>
-    <t>DAY 7</t>
-  </si>
-  <si>
-    <t>DAY 8</t>
-  </si>
-  <si>
-    <t>DAY 9</t>
+    <t>DAY 6 15-12-2025 (MONDAY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAY 7 </t>
   </si>
 </sst>
 </file>
@@ -841,11 +835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD51" sqref="AD51"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1067,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1123,7 +1117,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1158,392 +1152,374 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="4">
         <v>2776</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>2781</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="4">
         <v>2821</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="4">
         <v>2826</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="4" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>2831</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="A32" s="4">
+        <v>2836</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>2831</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" t="s">
-        <v>69</v>
+      <c r="A33" s="4">
+        <v>2889</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>2836</v>
+        <v>2894</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>2889</v>
+        <v>2899</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="A36">
+        <v>2933</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>2894</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" t="s">
-        <v>78</v>
-      </c>
+      <c r="A37" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>2899</v>
+        <v>3047</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>2933</v>
+        <v>3052</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="A40">
+        <v>3057</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>3047</v>
+        <v>3063</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>3052</v>
+        <v>3151</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" t="s">
-        <v>90</v>
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>3057</v>
+        <v>3157</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3063</v>
+        <v>3161</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>3151</v>
+        <v>3166</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>128</v>
+        <v>106</v>
+      </c>
+      <c r="D45" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3157</v>
+        <v>3371</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>3161</v>
+        <v>3376</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3166</v>
+        <v>3381</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>3371</v>
+        <v>3386</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>3376</v>
+        <v>3391</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" t="s">
-        <v>113</v>
+        <v>121</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>3381</v>
+        <v>3501</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D51" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>3386</v>
+        <v>3519</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>3391</v>
-      </c>
-      <c r="B53" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" t="s">
-        <v>121</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>3501</v>
-      </c>
-      <c r="B54" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>3519</v>
-      </c>
-      <c r="B55" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A40:D40"/>
+  <mergeCells count="6">
+    <mergeCell ref="A37:D37"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A14:D14"/>
@@ -1551,23 +1527,19 @@
     <mergeCell ref="A27:D27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C22" r:id="rId1" xr:uid="{973FA2AB-5B5C-4987-8FB2-6B643FA252D5}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{470F6B75-D68B-4834-AADC-84973047EAAD}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{7B276D0A-04E1-480A-AFA9-D133EE5CA0C5}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{77F78965-EA0B-4010-89DD-12DBED376854}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{8A17582B-DD8F-44EA-8FBF-56DCE5378DF3}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{BD476DA1-C383-4354-900D-366E68059EA6}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{FDA71AD3-8181-4206-8669-02CCFEFDA06D}"/>
-    <hyperlink ref="C15" r:id="rId8" xr:uid="{629F1413-583F-4011-B5AF-C754CFFAF9B1}"/>
-    <hyperlink ref="C42" r:id="rId9" xr:uid="{4A50E26B-7CD0-4332-AECA-A8C6556B935A}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{396D1191-1CF6-4ABC-989D-D95C3B3AC7A6}"/>
-    <hyperlink ref="C20" r:id="rId11" xr:uid="{F8A3E13A-134D-43BE-BAA8-A2EF3F81C94F}"/>
-    <hyperlink ref="C21" r:id="rId12" xr:uid="{C6E8F136-FA0E-4564-A24D-59A64360B152}"/>
-    <hyperlink ref="C24" r:id="rId13" xr:uid="{04B6DD5F-DB53-47C3-8F30-6D5785DB4372}"/>
-    <hyperlink ref="C25" r:id="rId14" xr:uid="{EDFBE1F0-3CB5-4203-B679-0BA4B296FB6E}"/>
-    <hyperlink ref="C26" r:id="rId15" xr:uid="{7D1C5303-AE3A-4D3D-B54E-7524D4E7D353}"/>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{470F6B75-D68B-4834-AADC-84973047EAAD}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{7B276D0A-04E1-480A-AFA9-D133EE5CA0C5}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{77F78965-EA0B-4010-89DD-12DBED376854}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{8A17582B-DD8F-44EA-8FBF-56DCE5378DF3}"/>
+    <hyperlink ref="C10" r:id="rId5" xr:uid="{BD476DA1-C383-4354-900D-366E68059EA6}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{FDA71AD3-8181-4206-8669-02CCFEFDA06D}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{629F1413-583F-4011-B5AF-C754CFFAF9B1}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{396D1191-1CF6-4ABC-989D-D95C3B3AC7A6}"/>
+    <hyperlink ref="C31" r:id="rId9" xr:uid="{EEB9D754-1F8E-4F56-9454-24FF87652F9E}"/>
+    <hyperlink ref="C32" r:id="rId10" xr:uid="{A335F142-B2EE-4699-97C8-E8662D9A76ED}"/>
+    <hyperlink ref="C33" r:id="rId11" xr:uid="{A5F4F1B3-2238-4EA2-8449-19ED0A412350}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WEEK 2 DAY 2 TUESDAY 16-12-2025 Completed
</commit_message>
<xml_diff>
--- a/DS Recordings.xlsx
+++ b/DS Recordings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Tofik\Desktop\INTERNSHIP-BRAINYBEAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B230C871-C0CD-4BE4-874A-68FF6E986C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C168E481-3338-4620-AB67-F5DADD0AB241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>task_id</t>
   </si>
@@ -420,17 +420,6 @@
     <t>From predicting customer behavior to optimizing operations, machine learning is transforming industries. Our project, [Project Name], demonstrates how data-driven models can solve . Today, we’ll showcase our methodology, challenges, and how our model enhances efficiency and accuracy</t>
   </si>
   <si>
-    <t>Common scaling methods include:
-Standardization (Z-score normalization): Transforms data to have a mean of 0 and a standard deviation of 1.
-Normalization (Min-Max Scaling): Rescales data between 0 and 1.</t>
-  </si>
-  <si>
-    <t>A well-structured presentation includes:
-Introduction: Briefly introduce the topic and purpose.
-Main Content: Explain key points with visuals.
-Conclusion: Summarize findings and provide takeaways.</t>
-  </si>
-  <si>
     <t>DAY 3 10-12-2025 (WEDNESDAY)</t>
   </si>
   <si>
@@ -446,7 +435,16 @@
     <t>DAY 6 15-12-2025 (MONDAY)</t>
   </si>
   <si>
-    <t xml:space="preserve">DAY 7 </t>
+    <t>DAY 8</t>
+  </si>
+  <si>
+    <t>DAY 7  16-12-2025 (TUESDAY)</t>
+  </si>
+  <si>
+    <t>Common scaling methods include: Standardization (Z-score normalization): Transforms data to have a mean of 0 and a standard deviation of 1. Normalization (Min-Max Scaling): Rescales data between 0 and 1.</t>
+  </si>
+  <si>
+    <t>A well-structured presentation includes: Introduction: Briefly introduce the topic and purpose. Main Content: Explain key points with visuals. Conclusion: Summarize findings and provide takeaways.</t>
   </si>
 </sst>
 </file>
@@ -835,11 +833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:D33"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,7 +911,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1011,7 +1009,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1067,7 +1065,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1117,7 +1115,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1167,7 +1165,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -1258,268 +1256,277 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="4">
         <v>2894</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="4">
         <v>2899</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
         <v>2933</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="4">
         <v>3047</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="4">
         <v>3052</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="4">
         <v>3057</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>3063</v>
-      </c>
-      <c r="B41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" t="s">
-        <v>96</v>
-      </c>
+      <c r="A41" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
+        <v>3063</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>3151</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>97</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>3157</v>
-      </c>
-      <c r="B43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" t="s">
-        <v>101</v>
+      <c r="D43" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3161</v>
+        <v>3157</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>3166</v>
+        <v>3161</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3371</v>
+        <v>3166</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>3376</v>
+        <v>3371</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3381</v>
+        <v>3376</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D48" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
+        <v>3381</v>
+      </c>
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>3386</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>117</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>118</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A50">
+    <row r="51" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>3391</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>120</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>3501</v>
-      </c>
-      <c r="B51" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" t="s">
-        <v>124</v>
+      <c r="D51" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
+        <v>3501</v>
+      </c>
+      <c r="B52" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>3519</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>125</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>126</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A37:D37"/>
+  <mergeCells count="7">
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A36:D36"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A14:D14"/>
@@ -1535,11 +1542,8 @@
     <hyperlink ref="C12" r:id="rId6" xr:uid="{FDA71AD3-8181-4206-8669-02CCFEFDA06D}"/>
     <hyperlink ref="C15" r:id="rId7" xr:uid="{629F1413-583F-4011-B5AF-C754CFFAF9B1}"/>
     <hyperlink ref="C11" r:id="rId8" xr:uid="{396D1191-1CF6-4ABC-989D-D95C3B3AC7A6}"/>
-    <hyperlink ref="C31" r:id="rId9" xr:uid="{EEB9D754-1F8E-4F56-9454-24FF87652F9E}"/>
-    <hyperlink ref="C32" r:id="rId10" xr:uid="{A335F142-B2EE-4699-97C8-E8662D9A76ED}"/>
-    <hyperlink ref="C33" r:id="rId11" xr:uid="{A5F4F1B3-2238-4EA2-8449-19ED0A412350}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>